<commit_message>
Changes to the Model to allow user to specify the column numbers of each required variable in each file.
</commit_message>
<xml_diff>
--- a/Vietnam_Production_Data.xlsx
+++ b/Vietnam_Production_Data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mathworks-my.sharepoint.com/personal/aredfear_mathworks_com/Documents/Work/CSE/Projects/SHAPE_APP_Andrew/Andrews Work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mathworks-my.sharepoint.com/personal/aredfear_mathworks_com/Documents/Work/CSE/Projects/SHAppE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_B359E617CF595FDA216121F1E3442AF07100E74F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9F9460A-4DBE-4950-9909-7A7074434B29}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_B359E617CF595FDA216121F1E3442AF07100E74F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DAA757D-42DC-4AF2-86CF-18F8E418FEA4}"/>
   <bookViews>
-    <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18600" yWindow="11289" windowWidth="18686" windowHeight="16542" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -407,11 +407,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="46.921875" customWidth="1"/>
+    <col min="1" max="1" width="20.69140625" customWidth="1"/>
     <col min="2" max="2" width="12.3046875" customWidth="1"/>
     <col min="3" max="3" width="8.84375" customWidth="1"/>
   </cols>

</xml_diff>